<commit_message>
adding two new sections to my application tracker
</commit_message>
<xml_diff>
--- a/2023_04_08_sub_F32/F32_progress_workbook.xlsx
+++ b/2023_04_08_sub_F32/F32_progress_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackdesmarais/Documents/Kinney_lab/Fellowships/2023_04_08_sub_F32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4412F426-22F6-7A41-B4DD-0B07470A796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BD4B6B-F4F8-E946-8EA1-AC5E6A6BE26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2500" windowWidth="28040" windowHeight="16600" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
+    <workbookView xWindow="41200" yWindow="6100" windowWidth="28040" windowHeight="16600" xr2:uid="{530E20B9-5E3F-674C-AD57-99FB2E7768B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Drafted</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>filling in (me)</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>equiptment</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -185,8 +194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}" name="Table1" displayName="Table1" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17" xr:uid="{F9D1F721-3EBE-0345-9CBA-2847C15A969F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{924DD312-80E3-224B-846B-36D22BCE72F7}" name="Section of Application"/>
     <tableColumn id="2" xr3:uid="{6EC5F282-D866-A543-8965-2A4B2374BA62}" name="Page Limits"/>
@@ -494,15 +503,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A7C2F5-51DA-C347-BCB0-CFA75EBC1137}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="150.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -553,154 +562,170 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>45018</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45003</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>45017</v>
+        <v>45018</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" s="1">
+        <v>45003</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45017</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C17" s="1">
         <v>45010</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>